<commit_message>
verizon test with data providers
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C21AF-09F0-4FED-B6AC-AABBDAE9B7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C2DC8D-D500-48B9-B5F1-53CF17036F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="2040" windowWidth="17280" windowHeight="8880" xr2:uid="{B50C9A9E-C94A-47A4-82EE-FD6F3A322C95}"/>
+    <workbookView xWindow="924" yWindow="2040" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{B50C9A9E-C94A-47A4-82EE-FD6F3A322C95}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectedCharger" sheetId="1" r:id="rId1"/>
+    <sheet name="LogInWithInvalidCredentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Verizon Car Adapter 40W USB-A and USB-C</t>
   </si>
   <si>
     <t>Verizon Car Adapter 45W USB-C Fast Charger</t>
+  </si>
+  <si>
+    <t>One or more of the values you have entered is incorrect.</t>
+  </si>
+  <si>
+    <t>sdofbgosdv</t>
+  </si>
+  <si>
+    <t>sdvjvblvds</t>
+  </si>
+  <si>
+    <t>43r9u34</t>
+  </si>
+  <si>
+    <t>&amp;^%$&amp;</t>
+  </si>
+  <si>
+    <t>&amp;^%&amp;*&amp;</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>34875832</t>
   </si>
 </sst>
 </file>
@@ -77,8 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869A3BEE-118E-4501-94CB-DC86E25017F4}">
   <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -415,4 +448,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84ADD58-1476-41C5-A563-F3ACA0B6993B}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
verizon. location search test
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C2DC8D-D500-48B9-B5F1-53CF17036F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDE11AD-A56C-495B-80B4-04974FF6A502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="2040" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{B50C9A9E-C94A-47A4-82EE-FD6F3A322C95}"/>
+    <workbookView xWindow="924" yWindow="2040" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{B50C9A9E-C94A-47A4-82EE-FD6F3A322C95}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectedCharger" sheetId="1" r:id="rId1"/>
     <sheet name="LogInWithInvalidCredentials" sheetId="2" r:id="rId2"/>
+    <sheet name="StoreLocator" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Verizon Car Adapter 40W USB-A and USB-C</t>
   </si>
@@ -73,6 +74,9 @@
   </si>
   <si>
     <t>34875832</t>
+  </si>
+  <si>
+    <t>11209</t>
   </si>
 </sst>
 </file>
@@ -454,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84ADD58-1476-41C5-A563-F3ACA0B6993B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -506,4 +510,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E484D48-7EF4-4898-8873-B8BF316B7A43}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>